<commit_message>
Fixed some ANOVAs & finished ranovas for all models except urban sites w/glmer
</commit_message>
<xml_diff>
--- a/Figures_Tables/ANOVA_tables_images/Model_List_annotated.xlsx
+++ b/Figures_Tables/ANOVA_tables_images/Model_List_annotated.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbrei\Documents\R_Projects\chapter_two\Figures_Tables\ANOVA_tables_images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{449231A3-D9A1-482F-AB51-2D3739B0CBB1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAC7B470-BCD6-4B30-9075-FEF5FC295F19}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="8604" yWindow="1272" windowWidth="13068" windowHeight="9504" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model_List" sheetId="1" r:id="rId1"/>
@@ -331,9 +331,6 @@
     <t>herb2020_urb_dist_m8_ME</t>
   </si>
   <si>
-    <t>~, log(Herbivory.Sept_mean), (1 | Block) + (1 | Population/Family) + City_dist + Transect_ID</t>
-  </si>
-  <si>
     <t>herb2020_urb_usc_m5</t>
   </si>
   <si>
@@ -626,14 +623,17 @@
   </si>
   <si>
     <t>R2m(delta)</t>
+  </si>
+  <si>
+    <t>~, log(Herbivory.July_mean), (1 | Block) + (1 | Population/Family) + City_dist + Transect_ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -1122,10 +1122,10 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="170" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1171,17 +1171,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1511,18 +1501,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView tabSelected="1" topLeftCell="C33" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="84.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" customWidth="1"/>
     <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.21875" style="3" bestFit="1" customWidth="1"/>
@@ -1540,13 +1530,13 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>199</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -1560,7 +1550,7 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -1576,7 +1566,7 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
@@ -1592,7 +1582,7 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
@@ -1608,7 +1598,7 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
@@ -1624,7 +1614,7 @@
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
@@ -1640,7 +1630,7 @@
         <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
@@ -1656,7 +1646,7 @@
         <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E8" s="1">
         <v>1</v>
@@ -1679,7 +1669,7 @@
         <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -1695,7 +1685,7 @@
         <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
@@ -1711,7 +1701,7 @@
         <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
@@ -1727,7 +1717,7 @@
         <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
@@ -1743,7 +1733,7 @@
         <v>26</v>
       </c>
       <c r="D13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
@@ -1759,7 +1749,7 @@
         <v>28</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E14" s="1">
         <v>1</v>
@@ -1782,7 +1772,7 @@
         <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
@@ -1798,7 +1788,7 @@
         <v>32</v>
       </c>
       <c r="D16" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
@@ -1814,7 +1804,7 @@
         <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
@@ -1830,7 +1820,7 @@
         <v>36</v>
       </c>
       <c r="D18" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
@@ -1846,7 +1836,7 @@
         <v>38</v>
       </c>
       <c r="D19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
@@ -1862,7 +1852,7 @@
         <v>40</v>
       </c>
       <c r="D20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
@@ -1878,7 +1868,7 @@
         <v>42</v>
       </c>
       <c r="D21" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
@@ -1894,7 +1884,7 @@
         <v>44</v>
       </c>
       <c r="D22" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
@@ -1910,7 +1900,7 @@
         <v>46</v>
       </c>
       <c r="D23" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
@@ -1926,7 +1916,7 @@
         <v>48</v>
       </c>
       <c r="D24" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
@@ -1942,7 +1932,7 @@
         <v>50</v>
       </c>
       <c r="D25" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
@@ -1958,7 +1948,7 @@
         <v>52</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E26" s="1">
         <v>1</v>
@@ -1981,7 +1971,7 @@
         <v>54</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E27" s="1">
         <v>1</v>
@@ -2004,7 +1994,7 @@
         <v>56</v>
       </c>
       <c r="D28" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
@@ -2020,7 +2010,7 @@
         <v>58</v>
       </c>
       <c r="D29" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
@@ -2036,7 +2026,7 @@
         <v>60</v>
       </c>
       <c r="D30" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
@@ -2052,7 +2042,7 @@
         <v>62</v>
       </c>
       <c r="D31" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
@@ -2068,7 +2058,7 @@
         <v>64</v>
       </c>
       <c r="D32" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
@@ -2084,7 +2074,7 @@
         <v>66</v>
       </c>
       <c r="D33" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
@@ -2100,7 +2090,7 @@
         <v>68</v>
       </c>
       <c r="D34" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
@@ -2116,7 +2106,7 @@
         <v>70</v>
       </c>
       <c r="D35" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
@@ -2132,7 +2122,7 @@
         <v>72</v>
       </c>
       <c r="D36" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
@@ -2148,7 +2138,7 @@
         <v>74</v>
       </c>
       <c r="D37" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
@@ -2164,7 +2154,7 @@
         <v>76</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E38" s="1">
         <v>1</v>
@@ -2187,7 +2177,7 @@
         <v>78</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E39" s="1">
         <v>1</v>
@@ -2210,7 +2200,7 @@
         <v>80</v>
       </c>
       <c r="D40" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
@@ -2226,7 +2216,7 @@
         <v>82</v>
       </c>
       <c r="D41" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
@@ -2242,7 +2232,7 @@
         <v>84</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E42" s="1">
         <v>1</v>
@@ -2265,7 +2255,7 @@
         <v>86</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E43" s="1">
         <v>1</v>
@@ -2288,7 +2278,7 @@
         <v>88</v>
       </c>
       <c r="D44" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
@@ -2304,7 +2294,7 @@
         <v>90</v>
       </c>
       <c r="D45" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
@@ -2320,7 +2310,7 @@
         <v>92</v>
       </c>
       <c r="D46" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
@@ -2336,7 +2326,7 @@
         <v>94</v>
       </c>
       <c r="D47" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
@@ -2352,7 +2342,7 @@
         <v>96</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E48" s="1">
         <v>1</v>
@@ -2375,7 +2365,7 @@
         <v>98</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E49" s="1">
         <v>1</v>
@@ -2398,7 +2388,7 @@
         <v>100</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E50" s="1">
         <v>1</v>
@@ -2411,33 +2401,40 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51">
+      <c r="A51" s="1">
         <v>50</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C51" t="s">
-        <v>102</v>
-      </c>
-      <c r="D51" t="s">
-        <v>197</v>
-      </c>
-      <c r="F51" s="4"/>
-      <c r="G51" s="4"/>
+      <c r="C51" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E51" s="1">
+        <v>1</v>
+      </c>
+      <c r="F51" s="4">
+        <v>1.158929E-2</v>
+      </c>
+      <c r="G51" s="4">
+        <v>2.042857E-2</v>
+      </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="D52" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E52" s="1">
         <v>1</v>
@@ -2454,13 +2451,13 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="D53" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E53" s="1">
         <v>1</v>
@@ -2477,13 +2474,13 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
+        <v>106</v>
+      </c>
+      <c r="C54" t="s">
         <v>107</v>
       </c>
-      <c r="C54" t="s">
-        <v>108</v>
-      </c>
       <c r="D54" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F54" s="4"/>
       <c r="G54" s="4"/>
@@ -2493,13 +2490,13 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
+        <v>108</v>
+      </c>
+      <c r="C55" t="s">
         <v>109</v>
       </c>
-      <c r="C55" t="s">
-        <v>110</v>
-      </c>
       <c r="D55" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
@@ -2509,13 +2506,13 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="D56" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E56" s="1">
         <v>1</v>
@@ -2532,13 +2529,13 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
+        <v>112</v>
+      </c>
+      <c r="C57" t="s">
         <v>113</v>
       </c>
-      <c r="C57" t="s">
-        <v>114</v>
-      </c>
       <c r="D57" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F57" s="4"/>
       <c r="G57" s="4"/>
@@ -2548,13 +2545,13 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
+        <v>114</v>
+      </c>
+      <c r="C58" t="s">
         <v>115</v>
       </c>
-      <c r="C58" t="s">
-        <v>116</v>
-      </c>
       <c r="D58" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F58" s="4"/>
       <c r="G58" s="4"/>
@@ -2564,13 +2561,13 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
+        <v>116</v>
+      </c>
+      <c r="C59" t="s">
         <v>117</v>
       </c>
-      <c r="C59" t="s">
-        <v>118</v>
-      </c>
       <c r="D59" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F59" s="4"/>
       <c r="G59" s="4"/>
@@ -2580,13 +2577,13 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
+        <v>118</v>
+      </c>
+      <c r="C60" t="s">
         <v>119</v>
       </c>
-      <c r="C60" t="s">
-        <v>120</v>
-      </c>
       <c r="D60" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F60" s="4"/>
       <c r="G60" s="4"/>
@@ -2596,13 +2593,13 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
+        <v>120</v>
+      </c>
+      <c r="C61" t="s">
         <v>121</v>
       </c>
-      <c r="C61" t="s">
-        <v>122</v>
-      </c>
       <c r="D61" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F61" s="4"/>
       <c r="G61" s="4"/>
@@ -2612,13 +2609,13 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
+        <v>122</v>
+      </c>
+      <c r="C62" t="s">
         <v>123</v>
       </c>
-      <c r="C62" t="s">
-        <v>124</v>
-      </c>
       <c r="D62" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F62" s="4"/>
       <c r="G62" s="4"/>
@@ -2628,13 +2625,13 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
+        <v>124</v>
+      </c>
+      <c r="C63" t="s">
         <v>125</v>
       </c>
-      <c r="C63" t="s">
-        <v>126</v>
-      </c>
       <c r="D63" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F63" s="4"/>
       <c r="G63" s="4"/>
@@ -2644,13 +2641,13 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
+        <v>126</v>
+      </c>
+      <c r="C64" t="s">
         <v>127</v>
       </c>
-      <c r="C64" t="s">
-        <v>128</v>
-      </c>
       <c r="D64" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>
@@ -2660,13 +2657,13 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
+        <v>128</v>
+      </c>
+      <c r="C65" t="s">
         <v>129</v>
       </c>
-      <c r="C65" t="s">
-        <v>130</v>
-      </c>
       <c r="D65" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F65" s="4"/>
       <c r="G65" s="4"/>
@@ -2676,13 +2673,13 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
+        <v>130</v>
+      </c>
+      <c r="C66" t="s">
         <v>131</v>
       </c>
-      <c r="C66" t="s">
-        <v>132</v>
-      </c>
       <c r="D66" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F66" s="4"/>
       <c r="G66" s="4"/>
@@ -2692,13 +2689,13 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
+        <v>132</v>
+      </c>
+      <c r="C67" t="s">
         <v>133</v>
       </c>
-      <c r="C67" t="s">
-        <v>134</v>
-      </c>
       <c r="D67" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F67" s="4"/>
       <c r="G67" s="4"/>
@@ -2708,13 +2705,13 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
+        <v>134</v>
+      </c>
+      <c r="C68" t="s">
         <v>135</v>
       </c>
-      <c r="C68" t="s">
-        <v>136</v>
-      </c>
       <c r="D68" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F68" s="4"/>
       <c r="G68" s="4"/>
@@ -2724,13 +2721,13 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
+        <v>136</v>
+      </c>
+      <c r="C69" t="s">
         <v>137</v>
       </c>
-      <c r="C69" t="s">
-        <v>138</v>
-      </c>
       <c r="D69" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F69" s="4"/>
       <c r="G69" s="4"/>
@@ -2740,13 +2737,13 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
+        <v>138</v>
+      </c>
+      <c r="C70" t="s">
         <v>139</v>
       </c>
-      <c r="C70" t="s">
-        <v>140</v>
-      </c>
       <c r="D70" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F70" s="4"/>
       <c r="G70" s="4"/>
@@ -2756,13 +2753,13 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
+        <v>140</v>
+      </c>
+      <c r="C71" t="s">
         <v>141</v>
       </c>
-      <c r="C71" t="s">
-        <v>142</v>
-      </c>
       <c r="D71" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F71" s="4"/>
       <c r="G71" s="4"/>
@@ -2772,13 +2769,13 @@
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C72" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C72" s="1" t="s">
-        <v>144</v>
-      </c>
       <c r="D72" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E72" s="1">
         <v>1</v>
@@ -2795,13 +2792,13 @@
         <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C73" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C73" s="1" t="s">
-        <v>146</v>
-      </c>
       <c r="D73" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E73" s="1">
         <v>1</v>
@@ -2818,13 +2815,13 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
+        <v>146</v>
+      </c>
+      <c r="C74" t="s">
         <v>147</v>
       </c>
-      <c r="C74" t="s">
-        <v>148</v>
-      </c>
       <c r="D74" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F74" s="4"/>
       <c r="G74" s="4"/>
@@ -2834,13 +2831,13 @@
         <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C75" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C75" s="1" t="s">
-        <v>150</v>
-      </c>
       <c r="D75" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E75" s="1">
         <v>1</v>
@@ -2857,13 +2854,13 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
+        <v>150</v>
+      </c>
+      <c r="C76" t="s">
         <v>151</v>
       </c>
-      <c r="C76" t="s">
-        <v>152</v>
-      </c>
       <c r="D76" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F76" s="4"/>
       <c r="G76" s="4"/>
@@ -2873,13 +2870,13 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
+        <v>152</v>
+      </c>
+      <c r="C77" t="s">
         <v>153</v>
       </c>
-      <c r="C77" t="s">
-        <v>154</v>
-      </c>
       <c r="D77" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F77" s="4"/>
       <c r="G77" s="4"/>
@@ -2889,13 +2886,13 @@
         <v>77</v>
       </c>
       <c r="B78" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C78" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C78" s="1" t="s">
-        <v>156</v>
-      </c>
       <c r="D78" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E78" s="1">
         <v>1</v>
@@ -2912,13 +2909,13 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
+        <v>156</v>
+      </c>
+      <c r="C79" t="s">
         <v>157</v>
       </c>
-      <c r="C79" t="s">
-        <v>158</v>
-      </c>
       <c r="D79" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F79" s="4"/>
       <c r="G79" s="4"/>
@@ -2928,13 +2925,13 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
+        <v>158</v>
+      </c>
+      <c r="C80" t="s">
         <v>159</v>
       </c>
-      <c r="C80" t="s">
-        <v>160</v>
-      </c>
       <c r="D80" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F80" s="4"/>
       <c r="G80" s="4"/>
@@ -2944,13 +2941,13 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
+        <v>160</v>
+      </c>
+      <c r="C81" t="s">
         <v>161</v>
       </c>
-      <c r="C81" t="s">
-        <v>162</v>
-      </c>
       <c r="D81" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F81" s="4"/>
       <c r="G81" s="4"/>
@@ -2960,13 +2957,13 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
+        <v>162</v>
+      </c>
+      <c r="C82" t="s">
         <v>163</v>
       </c>
-      <c r="C82" t="s">
-        <v>164</v>
-      </c>
       <c r="D82" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F82" s="4"/>
       <c r="G82" s="4"/>
@@ -2976,13 +2973,13 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
+        <v>164</v>
+      </c>
+      <c r="C83" t="s">
         <v>165</v>
       </c>
-      <c r="C83" t="s">
-        <v>166</v>
-      </c>
       <c r="D83" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F83" s="4"/>
       <c r="G83" s="4"/>
@@ -2992,13 +2989,13 @@
         <v>83</v>
       </c>
       <c r="B84" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C84" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="C84" s="1" t="s">
-        <v>168</v>
-      </c>
       <c r="D84" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E84" s="1">
         <v>1</v>
@@ -3015,13 +3012,13 @@
         <v>84</v>
       </c>
       <c r="B85" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C85" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="C85" s="1" t="s">
-        <v>170</v>
-      </c>
       <c r="D85" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E85" s="1">
         <v>1</v>
@@ -3038,13 +3035,13 @@
         <v>85</v>
       </c>
       <c r="B86" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C86" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="C86" s="1" t="s">
-        <v>172</v>
-      </c>
       <c r="D86" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E86" s="1">
         <v>1</v>
@@ -3061,13 +3058,13 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
+        <v>172</v>
+      </c>
+      <c r="C87" t="s">
         <v>173</v>
       </c>
-      <c r="C87" t="s">
-        <v>174</v>
-      </c>
       <c r="D87" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F87" s="4"/>
       <c r="G87" s="4"/>
@@ -3077,13 +3074,13 @@
         <v>87</v>
       </c>
       <c r="B88" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C88" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C88" s="1" t="s">
-        <v>176</v>
-      </c>
       <c r="D88" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E88" s="1">
         <v>1</v>
@@ -3100,13 +3097,13 @@
         <v>88</v>
       </c>
       <c r="B89" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C89" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C89" s="1" t="s">
-        <v>178</v>
-      </c>
       <c r="D89" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E89" s="1">
         <v>1</v>
@@ -3123,13 +3120,13 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
+        <v>178</v>
+      </c>
+      <c r="C90" t="s">
         <v>179</v>
       </c>
-      <c r="C90" t="s">
-        <v>180</v>
-      </c>
       <c r="D90" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F90" s="4"/>
       <c r="G90" s="4"/>
@@ -3139,13 +3136,13 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
+        <v>180</v>
+      </c>
+      <c r="C91" t="s">
         <v>181</v>
       </c>
-      <c r="C91" t="s">
-        <v>182</v>
-      </c>
       <c r="D91" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F91" s="4"/>
       <c r="G91" s="4"/>
@@ -3155,13 +3152,13 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
+        <v>182</v>
+      </c>
+      <c r="C92" t="s">
         <v>183</v>
       </c>
-      <c r="C92" t="s">
-        <v>184</v>
-      </c>
       <c r="D92" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F92" s="4"/>
       <c r="G92" s="4"/>
@@ -3171,13 +3168,13 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
+        <v>184</v>
+      </c>
+      <c r="C93" t="s">
         <v>185</v>
       </c>
-      <c r="C93" t="s">
-        <v>186</v>
-      </c>
       <c r="D93" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F93" s="4"/>
       <c r="G93" s="4"/>
@@ -3187,13 +3184,13 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
+        <v>186</v>
+      </c>
+      <c r="C94" t="s">
         <v>187</v>
       </c>
-      <c r="C94" t="s">
-        <v>188</v>
-      </c>
       <c r="D94" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F94" s="4"/>
       <c r="G94" s="4"/>
@@ -3203,13 +3200,13 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
+        <v>188</v>
+      </c>
+      <c r="C95" t="s">
         <v>189</v>
       </c>
-      <c r="C95" t="s">
-        <v>190</v>
-      </c>
       <c r="D95" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F95" s="4"/>
       <c r="G95" s="4"/>
@@ -3219,13 +3216,13 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
+        <v>190</v>
+      </c>
+      <c r="C96" t="s">
         <v>191</v>
       </c>
-      <c r="C96" t="s">
-        <v>192</v>
-      </c>
       <c r="D96" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F96" s="4"/>
       <c r="G96" s="4"/>
@@ -3235,24 +3232,24 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
+        <v>192</v>
+      </c>
+      <c r="C97" t="s">
         <v>193</v>
       </c>
-      <c r="C97" t="s">
-        <v>194</v>
-      </c>
       <c r="D97" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F97" s="4"/>
       <c r="G97" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="E1:E97"/>
+  <autoFilter ref="E1:E97" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="F1:F1048576">
     <cfRule type="expression" priority="3">
       <formula>$F:$F &gt; 0.1</formula>
     </cfRule>
-    <cfRule type="top10" dxfId="2" priority="2" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="1" priority="2" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">
     <cfRule type="top10" dxfId="0" priority="1" percent="1" rank="10"/>

</xml_diff>

<commit_message>
Made functions to find percent change along gradient and between urban subtransects
</commit_message>
<xml_diff>
--- a/Figures_Tables/ANOVA_tables_images/Model_List_annotated.xlsx
+++ b/Figures_Tables/ANOVA_tables_images/Model_List_annotated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbrei\Documents\R_Projects\chapter_two\Figures_Tables\ANOVA_tables_images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAC7B470-BCD6-4B30-9075-FEF5FC295F19}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E3C34F-0C6B-4808-B8BC-40D947DC1CDE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8604" yWindow="1272" windowWidth="13068" windowHeight="9504" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18144" yWindow="3000" windowWidth="9384" windowHeight="9504" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model_List" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="208">
   <si>
     <t>Model_Name1</t>
   </si>
@@ -626,6 +626,27 @@
   </si>
   <si>
     <t>~, log(Herbivory.July_mean), (1 | Block) + (1 | Population/Family) + City_dist + Transect_ID</t>
+  </si>
+  <si>
+    <t>Significant effect</t>
+  </si>
+  <si>
+    <t>City_dist</t>
+  </si>
+  <si>
+    <t>Transect_ID</t>
+  </si>
+  <si>
+    <t>Urb_score</t>
+  </si>
+  <si>
+    <t>City_dist &amp; Transect_ID</t>
+  </si>
+  <si>
+    <t>Interaction</t>
+  </si>
+  <si>
+    <t>Urb_score &amp; Transect_ID</t>
   </si>
 </sst>
 </file>
@@ -1502,24 +1523,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G97"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:H122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C33" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" customWidth="1"/>
-    <col min="3" max="3" width="27.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29.44140625" customWidth="1"/>
+    <col min="3" max="3" width="84.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" customWidth="1"/>
     <col min="6" max="6" width="9.21875" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1538,8 +1561,11 @@
       <c r="G1" s="3" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1555,7 +1581,7 @@
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1571,7 +1597,7 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1587,7 +1613,7 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1603,7 +1629,7 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1619,7 +1645,7 @@
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1635,7 +1661,7 @@
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1657,8 +1683,11 @@
       <c r="G8" s="5">
         <v>0.1381252</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H8" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1674,7 +1703,7 @@
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1690,7 +1719,7 @@
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1706,7 +1735,7 @@
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1722,7 +1751,7 @@
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1738,7 +1767,7 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1760,8 +1789,11 @@
       <c r="G14" s="2">
         <v>8.5808499999999996E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1777,7 +1809,7 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1793,7 +1825,7 @@
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1809,7 +1841,7 @@
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1825,7 +1857,7 @@
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1841,7 +1873,7 @@
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1857,7 +1889,7 @@
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1873,7 +1905,7 @@
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1889,7 +1921,7 @@
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1905,7 +1937,7 @@
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1921,7 +1953,7 @@
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1937,7 +1969,7 @@
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1959,8 +1991,11 @@
       <c r="G26" s="2">
         <v>7.9345390000000002E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H26" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1982,8 +2017,11 @@
       <c r="G27" s="2">
         <v>7.7327580000000007E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H27" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1999,7 +2037,7 @@
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2015,7 +2053,7 @@
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2031,7 +2069,7 @@
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2047,7 +2085,7 @@
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2063,7 +2101,7 @@
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2079,7 +2117,7 @@
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2095,7 +2133,7 @@
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2111,7 +2149,7 @@
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2127,7 +2165,7 @@
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2143,7 +2181,7 @@
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -2165,8 +2203,11 @@
       <c r="G38" s="2">
         <v>5.3068770000000001E-2</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H38" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -2188,8 +2229,11 @@
       <c r="G39" s="2">
         <v>5.2465329999999998E-2</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H39" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2205,7 +2249,7 @@
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2221,7 +2265,7 @@
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -2243,8 +2287,11 @@
       <c r="G42" s="2">
         <v>5.3042010000000001E-2</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H42" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -2266,8 +2313,11 @@
       <c r="G43" s="2">
         <v>5.2271970000000001E-2</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H43" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2283,7 +2333,7 @@
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2299,7 +2349,7 @@
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2315,7 +2365,7 @@
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2331,7 +2381,7 @@
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -2353,8 +2403,11 @@
       <c r="G48" s="2">
         <v>3.4089929999999997E-2</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H48" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -2376,8 +2429,11 @@
       <c r="G49" s="2">
         <v>3.2867359999999998E-2</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H49" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -2399,8 +2455,11 @@
       <c r="G50" s="2">
         <v>2.2178110000000001E-2</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H50" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -2422,8 +2481,11 @@
       <c r="G51" s="4">
         <v>2.042857E-2</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H51" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -2445,8 +2507,11 @@
       <c r="G52" s="2">
         <v>3.3872289999999999E-2</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H52" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -2468,8 +2533,11 @@
       <c r="G53" s="2">
         <v>3.3553970000000002E-2</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H53" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2485,7 +2553,7 @@
       <c r="F54" s="4"/>
       <c r="G54" s="4"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2501,7 +2569,7 @@
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -2523,8 +2591,11 @@
       <c r="G56" s="2">
         <v>1.3497810000000001E-2</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H56" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2540,7 +2611,7 @@
       <c r="F57" s="4"/>
       <c r="G57" s="4"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2556,7 +2627,7 @@
       <c r="F58" s="4"/>
       <c r="G58" s="4"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2572,7 +2643,7 @@
       <c r="F59" s="4"/>
       <c r="G59" s="4"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2588,7 +2659,7 @@
       <c r="F60" s="4"/>
       <c r="G60" s="4"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2604,7 +2675,7 @@
       <c r="F61" s="4"/>
       <c r="G61" s="4"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2620,7 +2691,7 @@
       <c r="F62" s="4"/>
       <c r="G62" s="4"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2636,7 +2707,7 @@
       <c r="F63" s="4"/>
       <c r="G63" s="4"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2652,7 +2723,7 @@
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2668,7 +2739,7 @@
       <c r="F65" s="4"/>
       <c r="G65" s="4"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2684,7 +2755,7 @@
       <c r="F66" s="4"/>
       <c r="G66" s="4"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2700,7 +2771,7 @@
       <c r="F67" s="4"/>
       <c r="G67" s="4"/>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2716,7 +2787,7 @@
       <c r="F68" s="4"/>
       <c r="G68" s="4"/>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
@@ -2732,7 +2803,7 @@
       <c r="F69" s="4"/>
       <c r="G69" s="4"/>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
@@ -2748,7 +2819,7 @@
       <c r="F70" s="4"/>
       <c r="G70" s="4"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2764,7 +2835,7 @@
       <c r="F71" s="4"/>
       <c r="G71" s="4"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -2786,8 +2857,11 @@
       <c r="G72" s="2">
         <v>3.9780570000000001E-2</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H72" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -2809,8 +2883,11 @@
       <c r="G73" s="2">
         <v>3.8458249999999999E-2</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H73" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>73</v>
       </c>
@@ -2826,7 +2903,7 @@
       <c r="F74" s="4"/>
       <c r="G74" s="4"/>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -2848,8 +2925,11 @@
       <c r="G75" s="2">
         <v>2.5593129999999999E-2</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H75" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>75</v>
       </c>
@@ -2865,7 +2945,7 @@
       <c r="F76" s="4"/>
       <c r="G76" s="4"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>76</v>
       </c>
@@ -2881,7 +2961,7 @@
       <c r="F77" s="4"/>
       <c r="G77" s="4"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -2903,8 +2983,11 @@
       <c r="G78" s="2">
         <v>2.5143240000000001E-2</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H78" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>78</v>
       </c>
@@ -2920,7 +3003,7 @@
       <c r="F79" s="4"/>
       <c r="G79" s="4"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>79</v>
       </c>
@@ -2936,7 +3019,7 @@
       <c r="F80" s="4"/>
       <c r="G80" s="4"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>80</v>
       </c>
@@ -2952,7 +3035,7 @@
       <c r="F81" s="4"/>
       <c r="G81" s="4"/>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>81</v>
       </c>
@@ -2968,7 +3051,7 @@
       <c r="F82" s="4"/>
       <c r="G82" s="4"/>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>82</v>
       </c>
@@ -2984,7 +3067,7 @@
       <c r="F83" s="4"/>
       <c r="G83" s="4"/>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -3006,8 +3089,11 @@
       <c r="G84" s="2">
         <v>0.1694253</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H84" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -3029,8 +3115,11 @@
       <c r="G85" s="2">
         <v>0.17030770000000001</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H85" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -3052,8 +3141,11 @@
       <c r="G86" s="2">
         <v>1.1249623E-2</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H86" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>86</v>
       </c>
@@ -3069,7 +3161,7 @@
       <c r="F87" s="4"/>
       <c r="G87" s="4"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -3091,8 +3183,11 @@
       <c r="G88" s="2">
         <v>1.4076490000000001E-2</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H88" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -3114,8 +3209,11 @@
       <c r="G89" s="2">
         <v>1.29841E-2</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H89" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>89</v>
       </c>
@@ -3131,7 +3229,7 @@
       <c r="F90" s="4"/>
       <c r="G90" s="4"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>90</v>
       </c>
@@ -3147,7 +3245,7 @@
       <c r="F91" s="4"/>
       <c r="G91" s="4"/>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>91</v>
       </c>
@@ -3163,7 +3261,7 @@
       <c r="F92" s="4"/>
       <c r="G92" s="4"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>92</v>
       </c>
@@ -3179,7 +3277,7 @@
       <c r="F93" s="4"/>
       <c r="G93" s="4"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>93</v>
       </c>
@@ -3195,7 +3293,7 @@
       <c r="F94" s="4"/>
       <c r="G94" s="4"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>94</v>
       </c>
@@ -3211,7 +3309,7 @@
       <c r="F95" s="4"/>
       <c r="G95" s="4"/>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>95</v>
       </c>
@@ -3227,7 +3325,7 @@
       <c r="F96" s="4"/>
       <c r="G96" s="4"/>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>96</v>
       </c>
@@ -3243,13 +3341,91 @@
       <c r="F97" s="4"/>
       <c r="G97" s="4"/>
     </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C99" s="1"/>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C100" s="1"/>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C101" s="1"/>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C102" s="1"/>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C103" s="1"/>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C104" s="1"/>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C105" s="1"/>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C106" s="1"/>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C107" s="1"/>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C108" s="1"/>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C109" s="1"/>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C110" s="1"/>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C111" s="1"/>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C112" s="1"/>
+    </row>
+    <row r="113" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C113" s="1"/>
+    </row>
+    <row r="114" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C114" s="1"/>
+    </row>
+    <row r="115" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C115" s="1"/>
+    </row>
+    <row r="116" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C116" s="1"/>
+    </row>
+    <row r="117" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C117" s="1"/>
+    </row>
+    <row r="118" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C118" s="1"/>
+    </row>
+    <row r="119" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C119" s="1"/>
+    </row>
+    <row r="120" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C120" s="1"/>
+    </row>
+    <row r="121" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C121" s="1"/>
+    </row>
+    <row r="122" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C122" s="1"/>
+    </row>
   </sheetData>
-  <autoFilter ref="E1:E97" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="E1:E97" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="top10" dxfId="1" priority="2" percent="1" rank="10"/>
     <cfRule type="expression" priority="3">
       <formula>$F:$F &gt; 0.1</formula>
     </cfRule>
-    <cfRule type="top10" dxfId="1" priority="2" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">
     <cfRule type="top10" dxfId="0" priority="1" percent="1" rank="10"/>

</xml_diff>

<commit_message>
Exported more ANOVA tables as images
</commit_message>
<xml_diff>
--- a/Figures_Tables/ANOVA_tables_images/Model_List_annotated.xlsx
+++ b/Figures_Tables/ANOVA_tables_images/Model_List_annotated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbrei\Documents\R_Projects\chapter_two\Figures_Tables\ANOVA_tables_images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E3C34F-0C6B-4808-B8BC-40D947DC1CDE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D11FC7E-6489-4B53-AA69-5BC8FCA4539D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18144" yWindow="3000" windowWidth="9384" windowHeight="9504" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="432" yWindow="1140" windowWidth="13068" windowHeight="9504" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model_List" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,23 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Model_List!$E$1:$E$97</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="208">
   <si>
     <t>Model_Name1</t>
   </si>
@@ -1140,13 +1151,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1526,8 +1538,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:H122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1970,30 +1982,24 @@
       <c r="G25" s="4"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="1">
+      <c r="A26" s="6">
         <v>25</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E26" s="1">
-        <v>1</v>
-      </c>
-      <c r="F26" s="2">
-        <v>1.148647E-2</v>
-      </c>
-      <c r="G26" s="2">
-        <v>7.9345390000000002E-2</v>
-      </c>
-      <c r="H26" t="s">
-        <v>203</v>
-      </c>
+      <c r="D26" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="E26" s="6">
+        <v>0</v>
+      </c>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="6"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="1">

</xml_diff>